<commit_message>
updated gender plots + employment data
Added 2020 to the employment data
Added/updated figures as discussed (only as png)
</commit_message>
<xml_diff>
--- a/1_data/akademisches_unibas.xlsx
+++ b/1_data/akademisches_unibas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Documents/CDS Group/CDS Brown Bag/Diversity_hackathon/1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB30186-D423-DE40-9D0D-D87161D548F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31647D33-3557-A942-9D0C-0524B9E03DBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
   <si>
     <t>Phil.-Hist. Fakultät</t>
   </si>
@@ -178,13 +178,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,55 +466,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P38"/>
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>2013</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9">
         <v>2014</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
         <v>2015</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9">
         <v>2016</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11">
+      <c r="J3" s="9"/>
+      <c r="K3" s="9">
         <v>2017</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11">
+      <c r="L3" s="9"/>
+      <c r="M3" s="9">
         <v>2018</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11">
+      <c r="N3" s="9"/>
+      <c r="O3" s="9">
         <v>2019</v>
       </c>
-      <c r="P3" s="11"/>
-    </row>
-    <row r="4" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9">
+        <v>2020</v>
+      </c>
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -561,8 +565,14 @@
       <c r="P4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -611,8 +621,14 @@
       <c r="P5" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="4">
+        <v>26</v>
+      </c>
+      <c r="R5" s="4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -659,8 +675,14 @@
       <c r="P6" s="4">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="4">
+        <v>36</v>
+      </c>
+      <c r="R6" s="4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -709,8 +731,14 @@
       <c r="P7" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="4">
+        <v>203</v>
+      </c>
+      <c r="R7" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -757,8 +785,14 @@
       <c r="P8" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="4">
+        <v>173</v>
+      </c>
+      <c r="R8" s="4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -777,8 +811,10 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -827,8 +863,14 @@
       <c r="P10" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q10" s="4">
+        <v>16</v>
+      </c>
+      <c r="R10" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -875,8 +917,14 @@
       <c r="P11" s="4">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="4">
+        <v>93</v>
+      </c>
+      <c r="R11" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -925,8 +973,14 @@
       <c r="P12" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="4">
+        <v>341</v>
+      </c>
+      <c r="R12" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>5</v>
@@ -973,14 +1027,20 @@
       <c r="P13" s="4">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="Q13" s="4">
+        <v>624</v>
+      </c>
+      <c r="R13" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -993,8 +1053,10 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1043,8 +1105,14 @@
       <c r="P15" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="4">
+        <v>26</v>
+      </c>
+      <c r="R15" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -1091,8 +1159,14 @@
       <c r="P16" s="4">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="4">
+        <v>98</v>
+      </c>
+      <c r="R16" s="4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -1141,8 +1215,14 @@
       <c r="P17" s="4">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="4">
+        <v>131</v>
+      </c>
+      <c r="R17" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
         <v>5</v>
@@ -1189,14 +1269,20 @@
       <c r="P18" s="4">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="Q18" s="4">
+        <v>148</v>
+      </c>
+      <c r="R18" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1209,8 +1295,10 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
@@ -1259,8 +1347,14 @@
       <c r="P20" s="4">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="4">
+        <v>6</v>
+      </c>
+      <c r="R20" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -1307,8 +1401,14 @@
       <c r="P21" s="4">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="4">
+        <v>11</v>
+      </c>
+      <c r="R21" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -1357,8 +1457,14 @@
       <c r="P22" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="4">
+        <v>22</v>
+      </c>
+      <c r="R22" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
         <v>5</v>
@@ -1405,13 +1511,19 @@
       <c r="P23" s="4">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="Q23" s="4">
+        <v>18</v>
+      </c>
+      <c r="R23" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1425,8 +1537,10 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
@@ -1475,8 +1589,14 @@
       <c r="P25" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="4">
+        <v>1</v>
+      </c>
+      <c r="R25" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1523,8 +1643,14 @@
       <c r="P26" s="4">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="4">
+        <v>9</v>
+      </c>
+      <c r="R26" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>6</v>
       </c>
@@ -1573,8 +1699,14 @@
       <c r="P27" s="4">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="4">
+        <v>55</v>
+      </c>
+      <c r="R27" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1621,13 +1753,19 @@
       <c r="P28" s="4">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="Q28" s="4">
+        <v>32</v>
+      </c>
+      <c r="R28" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1641,8 +1779,10 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -1691,8 +1831,14 @@
       <c r="P30" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q30" s="4">
+        <v>2</v>
+      </c>
+      <c r="R30" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1739,8 +1885,14 @@
       <c r="P31" s="4">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q31" s="4">
+        <v>8</v>
+      </c>
+      <c r="R31" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
@@ -1789,8 +1941,14 @@
       <c r="P32" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q32" s="4">
+        <v>20</v>
+      </c>
+      <c r="R32" s="4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1837,15 +1995,21 @@
       <c r="P33" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="Q33" s="4">
+        <v>15</v>
+      </c>
+      <c r="R33" s="4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -1857,8 +2021,10 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>3</v>
       </c>
@@ -1907,8 +2073,14 @@
       <c r="P35" s="4">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q35" s="4">
+        <v>6</v>
+      </c>
+      <c r="R35" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -1955,8 +2127,14 @@
       <c r="P36" s="4">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q36" s="4">
+        <v>20</v>
+      </c>
+      <c r="R36" s="4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
@@ -2005,8 +2183,14 @@
       <c r="P37" s="4">
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="4">
+        <v>29</v>
+      </c>
+      <c r="R37" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="3" t="s">
         <v>5</v>
@@ -2053,9 +2237,21 @@
       <c r="P38" s="4">
         <v>68</v>
       </c>
+      <c r="Q38" s="4">
+        <v>61</v>
+      </c>
+      <c r="R38" s="4">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
@@ -2063,11 +2259,6 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2076,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F646FA-1F51-5849-A3E9-B8C0CC370B45}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2088,7 +2279,7 @@
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -2116,8 +2307,11 @@
       <c r="I1" s="7">
         <v>2019</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2145,8 +2339,11 @@
       <c r="I2" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -2174,8 +2371,11 @@
       <c r="I3" s="7">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -2203,8 +2403,11 @@
       <c r="I4" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -2232,8 +2435,11 @@
       <c r="I5" s="7">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -2261,8 +2467,11 @@
       <c r="I6" s="7">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -2290,8 +2499,11 @@
       <c r="I7" s="7">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -2319,8 +2531,11 @@
       <c r="I8" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -2348,8 +2563,11 @@
       <c r="I9" s="7">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2377,8 +2595,11 @@
       <c r="I10" s="7">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -2406,8 +2627,11 @@
       <c r="I11" s="7">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -2435,8 +2659,11 @@
       <c r="I12" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -2464,8 +2691,11 @@
       <c r="I13" s="7">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2493,8 +2723,11 @@
       <c r="I14" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -2520,6 +2753,9 @@
         <v>33</v>
       </c>
       <c r="I15" s="7">
+        <v>32</v>
+      </c>
+      <c r="J15" s="7">
         <v>32</v>
       </c>
     </row>

</xml_diff>